<commit_message>
fixed damage property type fixed property: money->diamond
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/ConsumeData.xlsx
+++ b/_Out/NFDataCfg/Excel/ConsumeData.xlsx
@@ -53,9 +53,6 @@
     <t>Gold</t>
   </si>
   <si>
-    <t>Money</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>Force</t>
+  </si>
+  <si>
+    <t>Diamond</t>
   </si>
 </sst>
 </file>
@@ -794,7 +794,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -847,38 +847,38 @@
         <v>6</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1">
       <c r="A3" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1">
       <c r="A4" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1">
       <c r="A5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="9">
         <v>1</v>
@@ -956,7 +956,7 @@
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1">
       <c r="A6" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="9">
         <v>0</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1">
       <c r="A7" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1">
       <c r="A8" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1">
       <c r="A9" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -1060,33 +1060,33 @@
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1">
       <c r="A10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="C10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="G10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="H10" s="13" t="s">
         <v>21</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="16">
         <v>0</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="16">
         <v>100</v>
@@ -1138,7 +1138,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="16">
         <v>0</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="16">
         <v>0</v>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="16">
         <v>0</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="16">
         <v>0</v>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="16">
         <v>0</v>
@@ -1268,7 +1268,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="16">
         <v>0</v>
@@ -1294,7 +1294,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="16">
         <v>0</v>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="16">
         <v>0</v>
@@ -1346,7 +1346,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="16">
         <v>0</v>
@@ -1372,7 +1372,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="16">
         <v>0</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="16">
         <v>0</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="16">
         <v>0</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="16">
         <v>0</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="16">
         <v>0</v>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="16">
         <v>0</v>
@@ -1528,7 +1528,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="16">
         <v>0</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="16">
         <v>0</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="16">
         <v>0</v>
@@ -1606,7 +1606,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="16">
         <v>0</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" s="16">
         <v>0</v>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="16">
         <v>0</v>

</xml_diff>